<commit_message>
Added a column explicitly stating whether two events of a mutation are required in the gene.
</commit_message>
<xml_diff>
--- a/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
+++ b/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="37080" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Alascca table of mutation class" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="197">
   <si>
     <t>Gene</t>
   </si>
@@ -597,6 +597,21 @@
   </si>
   <si>
     <t>VEP Consequence types are SO terms described at http://www.ensembl.org/info/genome/variation/predicted_data.html#consequences</t>
+  </si>
+  <si>
+    <t>ENSG00000167244</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Two_Events_Required</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -697,7 +712,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="157">
+  <cellStyleXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -855,27 +870,26 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -905,13 +919,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="157">
+  <cellStyles count="165">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -990,6 +1004,10 @@
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1068,6 +1086,10 @@
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1085,8 +1107,8 @@
       <xdr:rowOff>80433</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>482705</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>152505</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>143932</xdr:rowOff>
     </xdr:to>
@@ -1463,15 +1485,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.1640625" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" customWidth="1"/>
-    <col min="7" max="7" width="7.5" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="99" style="6" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="19" customWidth="1"/>
+    <col min="6" max="6" width="40.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="5.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
@@ -1479,649 +1501,711 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="17"/>
+      <c r="D2" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>193</v>
+      </c>
       <c r="F2" s="14"/>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="14"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="F3" s="15"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="10" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="F5" s="15"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="10" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="F6" s="15"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="10" t="s">
         <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
+      <c r="F7" s="15"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
+      <c r="F8" s="15"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
+      <c r="F9" s="15"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="5"/>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="F10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="5"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="F11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="5"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="F12" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="5"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="23" t="s">
+        <v>196</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="F13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="5"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="F14" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="D15" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="E15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="F15" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="20"/>
+      <c r="H15" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="12"/>
-      <c r="I15" s="24"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="D16" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="E16" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="F16" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="20"/>
+      <c r="H16" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="24"/>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="F17" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="3"/>
+      <c r="H17" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="I17"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="F18" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="I18"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="F19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="I19"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="F20" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="3"/>
+      <c r="H20" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="D21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="E21" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="F21" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="6"/>
+      <c r="H21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="4"/>
+      <c r="I21"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="D22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="E22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="F22" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="6"/>
+      <c r="H22" s="7" t="s">
         <v>28</v>
       </c>
+      <c r="I22"/>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="11"/>
+      <c r="A43" s="8"/>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="11"/>
+      <c r="A44" s="8"/>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="11"/>
+      <c r="A45" s="8"/>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="11"/>
+      <c r="A46" s="8"/>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="11"/>
+      <c r="A47" s="8"/>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="11"/>
+      <c r="A48" s="8"/>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="11"/>
+      <c r="A49" s="8"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="11"/>
+      <c r="A50" s="8"/>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="11"/>
+      <c r="A51" s="8"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="11"/>
+      <c r="A52" s="8"/>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="11"/>
+      <c r="A53" s="8"/>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="11"/>
+      <c r="A54" s="8"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="11"/>
+      <c r="A55" s="8"/>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="11"/>
+      <c r="A56" s="8"/>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="11"/>
+      <c r="A57" s="8"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="11"/>
+      <c r="A58" s="8"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="11"/>
+      <c r="A59" s="8"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="11"/>
+      <c r="A60" s="8"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="11"/>
+      <c r="A61" s="8"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="11"/>
+      <c r="A62" s="8"/>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="11"/>
+      <c r="A63" s="8"/>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="11"/>
+      <c r="A64" s="8"/>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="11"/>
+      <c r="A65" s="8"/>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="11"/>
+      <c r="A66" s="8"/>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="11"/>
+      <c r="A67" s="8"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="11"/>
+      <c r="A68" s="8"/>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="11"/>
+      <c r="A69" s="8"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="11"/>
+      <c r="A70" s="8"/>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="11"/>
+      <c r="A71" s="8"/>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="11"/>
+      <c r="A72" s="8"/>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="11"/>
+      <c r="A73" s="8"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="11"/>
+      <c r="A74" s="8"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="11"/>
+      <c r="A75" s="8"/>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="11"/>
+      <c r="A76" s="8"/>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="11"/>
+      <c r="A77" s="8"/>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="11"/>
+      <c r="A78" s="8"/>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="11"/>
+      <c r="A79" s="8"/>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="11"/>
+      <c r="A80" s="8"/>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="11"/>
+      <c r="A81" s="8"/>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="11"/>
+      <c r="A82" s="8"/>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="11"/>
+      <c r="A83" s="8"/>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="11"/>
+      <c r="A84" s="8"/>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="11"/>
+      <c r="A85" s="8"/>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="11"/>
+      <c r="A86" s="8"/>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="11"/>
+      <c r="A87" s="8"/>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="11"/>
+      <c r="A88" s="8"/>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="11"/>
+      <c r="A89" s="8"/>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="11"/>
+      <c r="A90" s="8"/>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="11"/>
+      <c r="A91" s="8"/>
     </row>
     <row r="92" spans="1:1">
-      <c r="A92" s="11"/>
+      <c r="A92" s="8"/>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="11"/>
+      <c r="A93" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2173,7 +2257,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="22" t="s">
         <v>115</v>
       </c>
       <c r="B4" t="s">
@@ -2431,8 +2515,8 @@
       <c r="F13" t="s">
         <v>62</v>
       </c>
-      <c r="T13" s="25"/>
-      <c r="Z13" s="25"/>
+      <c r="T13" s="21"/>
+      <c r="Z13" s="21"/>
     </row>
     <row r="14" spans="1:26">
       <c r="B14" t="s">

</xml_diff>

<commit_message>
Minor changes to tables defining mutation rules. Preparing to implement report compilation tool.
</commit_message>
<xml_diff>
--- a/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
+++ b/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="37080" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Alascca table of mutation class" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="186">
   <si>
     <t>Gene</t>
   </si>
@@ -29,15 +29,6 @@
     <t>Feature</t>
   </si>
   <si>
-    <t>Protein_position</t>
-  </si>
-  <si>
-    <t>Amino_acids</t>
-  </si>
-  <si>
-    <t>SYMBOL</t>
-  </si>
-  <si>
     <t>Consequence</t>
   </si>
   <si>
@@ -53,30 +44,6 @@
     <t>ENST00000371953</t>
   </si>
   <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>C/S</t>
-  </si>
-  <si>
-    <t>129</t>
-  </si>
-  <si>
-    <t>G/E</t>
-  </si>
-  <si>
-    <t>130</t>
-  </si>
-  <si>
-    <t>R/G</t>
-  </si>
-  <si>
-    <t>R/Q</t>
-  </si>
-  <si>
-    <t>Class</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -599,13 +566,19 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Two_Events_Required</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Yes</t>
+    <t>C124S,G129E,R130G,R130Q</t>
+  </si>
+  <si>
+    <t>Amino_acid_changes</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>Number_Required</t>
+  </si>
+  <si>
+    <t>Flag</t>
   </si>
 </sst>
 </file>
@@ -706,7 +679,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="167">
+  <cellStyleXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -874,8 +847,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -888,7 +873,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -921,7 +905,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="167">
+  <cellStyles count="179">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1005,6 +989,12 @@
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1088,6 +1078,12 @@
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1101,13 +1097,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>169333</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>2502005</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:colOff>698605</xdr:colOff>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>42332</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1474,11 +1470,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1487,555 +1483,468 @@
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" style="17" customWidth="1"/>
-    <col min="6" max="6" width="40.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="8" width="5.33203125" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="9">
+        <v>1</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="2">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="2">
+        <v>2</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="12"/>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="2">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="2">
         <v>1</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="G8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="F10" s="20">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="21">
+        <v>1</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="21">
+        <v>1</v>
+      </c>
+      <c r="G12" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="21">
+        <v>1</v>
+      </c>
+      <c r="G13" s="17" t="s">
         <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9"/>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10"/>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>193</v>
+        <v>3</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="21">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="21">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="8"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="8"/>
+      <c r="B16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="21">
+        <v>1</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>193</v>
+        <v>24</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="21">
+        <v>1</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="I17"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3" t="s">
-        <v>18</v>
+      <c r="F18" s="22">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="I18"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3" t="s">
-        <v>18</v>
+      <c r="A19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="22">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="I19"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="I21"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="6" t="s">
-        <v>27</v>
-      </c>
       <c r="I22"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="7"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="7"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="7"/>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="7"/>
@@ -2180,15 +2089,6 @@
     </row>
     <row r="90" spans="1:1">
       <c r="A90" s="7"/>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="7"/>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="7"/>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2217,34 +2117,34 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="20" t="s">
-        <v>113</v>
+      <c r="A4" s="19" t="s">
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2277,624 +2177,624 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B1" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C1" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="D1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="E1" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F1" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:26">
       <c r="B2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="B3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="B4" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="B5" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="B6" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="F6" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="B7" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C7" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="B8" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="F8" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="B9" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="B10" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="B11" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:26">
       <c r="B12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D12" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="B13" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
-      </c>
-      <c r="T13" s="19"/>
-      <c r="Z13" s="19"/>
+        <v>49</v>
+      </c>
+      <c r="T13" s="18"/>
+      <c r="Z13" s="18"/>
     </row>
     <row r="14" spans="1:26">
       <c r="B14" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="D14" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="F14" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="B15" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="F15" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="B16" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E16" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="F16" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C17" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E17" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="F17" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="F18" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="F19" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C20" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="D20" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="F20" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="D21" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E21" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="F21" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E22" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="F22" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C23" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D23" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E23" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="F23" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="E24" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="F24" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="2:6">
       <c r="B25" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="E25" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="F25" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F26" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="C27" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D27" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="F27" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="D28" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E28" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F28" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C29" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D29" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="E29" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="F29" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D30" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E30" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="F30" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="D31" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="E31" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="F31" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C32" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="D32" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E32" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="F32" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="B33" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C33" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D33" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="E33" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="F33" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="B34" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C34" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D34" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="E34" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="F34" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="B35" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C35" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D35" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="E35" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="F35" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="B36" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C36" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D36" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E36" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="F36" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Collapsed flag and number required columns down into a single column (flag), so that the format of this mutation table is identical to the format of the colorectal mutations, in terms of columns required.
</commit_message>
<xml_diff>
--- a/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
+++ b/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="1020" yWindow="680" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Alascca table of mutation class" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="186">
   <si>
     <t>Gene</t>
   </si>
@@ -44,9 +44,6 @@
     <t>ENST00000371953</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>homozygous_loss</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>ENST00000263967</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>542,545,546,1021,1043,1044,1047</t>
   </si>
   <si>
@@ -575,10 +569,16 @@
     <t>Symbol</t>
   </si>
   <si>
-    <t>Number_Required</t>
-  </si>
-  <si>
     <t>Flag</t>
+  </si>
+  <si>
+    <t>ALASSCA_CLASS_B_1</t>
+  </si>
+  <si>
+    <t>ALASSCA_CLASS_A</t>
+  </si>
+  <si>
+    <t>ALASSCA_CLASS_B_2</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -669,6 +669,12 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -679,7 +685,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="179">
+  <cellStyleXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -859,8 +865,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -869,9 +883,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -899,13 +910,11 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="179">
+  <cellStyles count="187">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -995,6 +1004,10 @@
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1084,6 +1097,10 @@
     <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1474,7 +1491,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1483,9 +1500,10 @@
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.1640625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" customWidth="1"/>
-    <col min="7" max="8" width="5.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="20.5" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1494,7 +1512,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1502,41 +1520,35 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>185</v>
-      </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="9">
-        <v>1</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>7</v>
+      <c r="A2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="8" t="s">
+        <v>183</v>
       </c>
       <c r="I2"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="8" t="s">
-        <v>20</v>
+      <c r="A3" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
@@ -1547,18 +1559,15 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="2">
-        <v>2</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>7</v>
+      <c r="E3" s="11"/>
+      <c r="F3" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="I3"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="8" t="s">
-        <v>22</v>
+      <c r="A4" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
@@ -1569,18 +1578,15 @@
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="2">
-        <v>2</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>7</v>
+      <c r="E4" s="11"/>
+      <c r="F4" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="I4"/>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="8" t="s">
-        <v>25</v>
+      <c r="A5" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -1591,18 +1597,15 @@
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="2">
-        <v>2</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>7</v>
+      <c r="E5" s="11"/>
+      <c r="F5" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="I5"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="8" t="s">
-        <v>23</v>
+      <c r="A6" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -1613,18 +1616,15 @@
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="2">
-        <v>2</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>7</v>
+      <c r="E6" s="11"/>
+      <c r="F6" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="8" t="s">
-        <v>24</v>
+      <c r="A7" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -1635,18 +1635,15 @@
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="2">
-        <v>2</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>7</v>
+      <c r="E7" s="11"/>
+      <c r="F7" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="24" t="s">
-        <v>9</v>
+      <c r="A8" s="20" t="s">
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
@@ -1657,18 +1654,15 @@
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="E8" s="11"/>
+      <c r="F8" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="20" t="s">
         <v>7</v>
-      </c>
-      <c r="I8"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="24" t="s">
-        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>4</v>
@@ -1679,17 +1673,14 @@
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>7</v>
+      <c r="E9" s="11"/>
+      <c r="F9" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="I9"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1701,86 +1692,74 @@
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>181</v>
-      </c>
-      <c r="F10" s="20">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>7</v>
+      <c r="E10" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="I10"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="21">
-        <v>1</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="17" t="s">
+      <c r="B13" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="21">
-        <v>1</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12"/>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="21">
-        <v>1</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>7</v>
+      <c r="E13" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>183</v>
       </c>
       <c r="I13"/>
     </row>
@@ -1789,94 +1768,82 @@
         <v>3</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F14" s="21">
-        <v>1</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>7</v>
+      <c r="E14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>183</v>
       </c>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="21">
-        <v>1</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>7</v>
+      <c r="E15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>183</v>
       </c>
       <c r="I15"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="21">
-        <v>1</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>7</v>
+      <c r="E16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>183</v>
       </c>
       <c r="I16"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="21">
-        <v>1</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>7</v>
+      <c r="E17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>183</v>
       </c>
       <c r="I17"/>
     </row>
@@ -1885,22 +1852,19 @@
         <v>3</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="22">
-        <v>1</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>7</v>
+      <c r="E18" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>183</v>
       </c>
       <c r="I18"/>
     </row>
@@ -1909,22 +1873,19 @@
         <v>3</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="22">
-        <v>1</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>16</v>
+      <c r="F19" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="I19"/>
     </row>
@@ -1938,157 +1899,157 @@
       <c r="I22"/>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="7"/>
+      <c r="A40" s="6"/>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="7"/>
+      <c r="A41" s="6"/>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="7"/>
+      <c r="A42" s="6"/>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="7"/>
+      <c r="A43" s="6"/>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="7"/>
+      <c r="A44" s="6"/>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="7"/>
+      <c r="A45" s="6"/>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="7"/>
+      <c r="A46" s="6"/>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="7"/>
+      <c r="A47" s="6"/>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="7"/>
+      <c r="A48" s="6"/>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="7"/>
+      <c r="A49" s="6"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="7"/>
+      <c r="A50" s="6"/>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="7"/>
+      <c r="A51" s="6"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="7"/>
+      <c r="A52" s="6"/>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="7"/>
+      <c r="A53" s="6"/>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="7"/>
+      <c r="A54" s="6"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="7"/>
+      <c r="A55" s="6"/>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="7"/>
+      <c r="A56" s="6"/>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="7"/>
+      <c r="A57" s="6"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="7"/>
+      <c r="A58" s="6"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="7"/>
+      <c r="A59" s="6"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="7"/>
+      <c r="A60" s="6"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="7"/>
+      <c r="A61" s="6"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="7"/>
+      <c r="A62" s="6"/>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="7"/>
+      <c r="A63" s="6"/>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="7"/>
+      <c r="A64" s="6"/>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="7"/>
+      <c r="A65" s="6"/>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="7"/>
+      <c r="A66" s="6"/>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="7"/>
+      <c r="A67" s="6"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="7"/>
+      <c r="A68" s="6"/>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="7"/>
+      <c r="A69" s="6"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="7"/>
+      <c r="A70" s="6"/>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="7"/>
+      <c r="A71" s="6"/>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="7"/>
+      <c r="A72" s="6"/>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="7"/>
+      <c r="A73" s="6"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="7"/>
+      <c r="A74" s="6"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="7"/>
+      <c r="A75" s="6"/>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="7"/>
+      <c r="A76" s="6"/>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="7"/>
+      <c r="A77" s="6"/>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="7"/>
+      <c r="A78" s="6"/>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="7"/>
+      <c r="A79" s="6"/>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="7"/>
+      <c r="A80" s="6"/>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="7"/>
+      <c r="A81" s="6"/>
     </row>
     <row r="82" spans="1:1">
-      <c r="A82" s="7"/>
+      <c r="A82" s="6"/>
     </row>
     <row r="83" spans="1:1">
-      <c r="A83" s="7"/>
+      <c r="A83" s="6"/>
     </row>
     <row r="84" spans="1:1">
-      <c r="A84" s="7"/>
+      <c r="A84" s="6"/>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="7"/>
+      <c r="A85" s="6"/>
     </row>
     <row r="86" spans="1:1">
-      <c r="A86" s="7"/>
+      <c r="A86" s="6"/>
     </row>
     <row r="87" spans="1:1">
-      <c r="A87" s="7"/>
+      <c r="A87" s="6"/>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="7"/>
+      <c r="A88" s="6"/>
     </row>
     <row r="89" spans="1:1">
-      <c r="A89" s="7"/>
+      <c r="A89" s="6"/>
     </row>
     <row r="90" spans="1:1">
-      <c r="A90" s="7"/>
+      <c r="A90" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2117,34 +2078,34 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="19" t="s">
-        <v>102</v>
+      <c r="A4" s="18" t="s">
+        <v>100</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2177,192 +2138,192 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1" t="s">
         <v>172</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>173</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>174</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>175</v>
-      </c>
-      <c r="E1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:26">
       <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" t="s">
         <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>104</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="B4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="B7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="B9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="B10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -2370,431 +2331,431 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="B13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F13" t="s">
-        <v>49</v>
-      </c>
-      <c r="T13" s="18"/>
-      <c r="Z13" s="18"/>
+        <v>47</v>
+      </c>
+      <c r="T13" s="17"/>
+      <c r="Z13" s="17"/>
     </row>
     <row r="14" spans="1:26">
       <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" t="s">
         <v>54</v>
-      </c>
-      <c r="C14" t="s">
-        <v>127</v>
-      </c>
-      <c r="D14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" t="s">
-        <v>128</v>
-      </c>
-      <c r="F14" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="B15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="B16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" t="s">
+        <v>134</v>
+      </c>
+      <c r="F18" t="s">
         <v>63</v>
-      </c>
-      <c r="C18" t="s">
-        <v>135</v>
-      </c>
-      <c r="D18" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" t="s">
-        <v>136</v>
-      </c>
-      <c r="F18" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E21" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="2:6">
       <c r="B25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C25" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E26" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E27" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E28" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E29" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C30" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C32" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E32" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="B33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C33" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D33" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="B34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D34" t="s">
+        <v>94</v>
+      </c>
+      <c r="E34" t="s">
         <v>165</v>
       </c>
-      <c r="D34" t="s">
-        <v>96</v>
-      </c>
-      <c r="E34" t="s">
-        <v>167</v>
-      </c>
       <c r="F34" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="B35" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C35" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D35" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E35" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="B36" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C36" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E36" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Collapsed rows with identical fields but separate "consequence" values down into one row, with a list of consequence values provided.
</commit_message>
<xml_diff>
--- a/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
+++ b/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="680" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="1620" yWindow="300" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Alascca table of mutation class" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="187">
   <si>
     <t>Gene</t>
   </si>
@@ -44,12 +44,6 @@
     <t>ENST00000371953</t>
   </si>
   <si>
-    <t>homozygous_loss</t>
-  </si>
-  <si>
-    <t>loss_of_heterozygosity</t>
-  </si>
-  <si>
     <t>PIK3R1</t>
   </si>
   <si>
@@ -579,6 +573,15 @@
   </si>
   <si>
     <t>ALASSCA_CLASS_B_2</t>
+  </si>
+  <si>
+    <t>start_lost,stop_gained,frameshift_variant,splice_acceptor_variant,splice_donor_variant</t>
+  </si>
+  <si>
+    <t>loss_of_heterozygosity,homozygous_loss</t>
+  </si>
+  <si>
+    <t>frameshift_variant,inframe_insertion,inframe_deletion,stop_gained,splice_acceptor_variant,splice_donor_variant</t>
   </si>
 </sst>
 </file>
@@ -632,7 +635,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -665,12 +668,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDAEEF3"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -685,7 +682,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="187">
+  <cellStyleXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -873,48 +870,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="187">
+  <cellStyles count="189">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1008,6 +1004,7 @@
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1101,6 +1098,7 @@
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1114,13 +1112,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>169333</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>698605</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>42332</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1487,24 +1485,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I90"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="94.6640625" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.1640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" style="5" customWidth="1"/>
     <col min="6" max="6" width="20.5" customWidth="1"/>
     <col min="7" max="7" width="5.33203125" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
@@ -1512,7 +1510,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1520,373 +1518,203 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="I5"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="I6"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="I2"/>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I3"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I4"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I5"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I6"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="I7"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="I8"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="I9"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="I10"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="21" t="s">
-        <v>183</v>
-      </c>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="21" t="s">
-        <v>183</v>
-      </c>
       <c r="I12"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>183</v>
-      </c>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>183</v>
-      </c>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="21" t="s">
-        <v>183</v>
-      </c>
       <c r="I15"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="21" t="s">
-        <v>183</v>
-      </c>
       <c r="I16"/>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="21" t="s">
-        <v>183</v>
-      </c>
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>183</v>
-      </c>
       <c r="I18"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>184</v>
-      </c>
       <c r="I19"/>
     </row>
     <row r="20" spans="1:9">
@@ -1898,158 +1726,158 @@
     <row r="22" spans="1:9">
       <c r="I22"/>
     </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="3"/>
+    </row>
+    <row r="31" spans="1:9">
+      <c r="A31" s="3"/>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="3"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="3"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="3"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="3"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="3"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="3"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="3"/>
+    </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="6"/>
+      <c r="A40" s="3"/>
     </row>
     <row r="41" spans="1:1">
-      <c r="A41" s="6"/>
+      <c r="A41" s="3"/>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="6"/>
+      <c r="A42" s="3"/>
     </row>
     <row r="43" spans="1:1">
-      <c r="A43" s="6"/>
+      <c r="A43" s="3"/>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="6"/>
+      <c r="A44" s="3"/>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="6"/>
+      <c r="A45" s="3"/>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="6"/>
+      <c r="A46" s="3"/>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="6"/>
+      <c r="A47" s="3"/>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="6"/>
+      <c r="A48" s="3"/>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="6"/>
+      <c r="A49" s="3"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="6"/>
+      <c r="A50" s="3"/>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="6"/>
+      <c r="A51" s="3"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="6"/>
+      <c r="A52" s="3"/>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="6"/>
+      <c r="A53" s="3"/>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="6"/>
+      <c r="A54" s="3"/>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="6"/>
+      <c r="A55" s="3"/>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="6"/>
+      <c r="A56" s="3"/>
     </row>
     <row r="57" spans="1:1">
-      <c r="A57" s="6"/>
+      <c r="A57" s="3"/>
     </row>
     <row r="58" spans="1:1">
-      <c r="A58" s="6"/>
+      <c r="A58" s="3"/>
     </row>
     <row r="59" spans="1:1">
-      <c r="A59" s="6"/>
+      <c r="A59" s="3"/>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="6"/>
+      <c r="A60" s="3"/>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="6"/>
+      <c r="A61" s="3"/>
     </row>
     <row r="62" spans="1:1">
-      <c r="A62" s="6"/>
+      <c r="A62" s="3"/>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="6"/>
+      <c r="A63" s="3"/>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="6"/>
+      <c r="A64" s="3"/>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="6"/>
+      <c r="A65" s="3"/>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="6"/>
+      <c r="A66" s="3"/>
     </row>
     <row r="67" spans="1:1">
-      <c r="A67" s="6"/>
+      <c r="A67" s="3"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="6"/>
+      <c r="A68" s="3"/>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="6"/>
+      <c r="A69" s="3"/>
     </row>
     <row r="70" spans="1:1">
-      <c r="A70" s="6"/>
+      <c r="A70" s="3"/>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="6"/>
+      <c r="A71" s="3"/>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="6"/>
+      <c r="A72" s="3"/>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="6"/>
+      <c r="A73" s="3"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="6"/>
+      <c r="A74" s="3"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="6"/>
+      <c r="A75" s="3"/>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="6"/>
+      <c r="A76" s="3"/>
     </row>
     <row r="77" spans="1:1">
-      <c r="A77" s="6"/>
+      <c r="A77" s="3"/>
     </row>
     <row r="78" spans="1:1">
-      <c r="A78" s="6"/>
+      <c r="A78" s="3"/>
     </row>
     <row r="79" spans="1:1">
-      <c r="A79" s="6"/>
+      <c r="A79" s="3"/>
     </row>
     <row r="80" spans="1:1">
-      <c r="A80" s="6"/>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" s="6"/>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" s="6"/>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" s="6"/>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" s="6"/>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" s="6"/>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="6"/>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="6"/>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" s="6"/>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" s="6"/>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" s="6"/>
+      <c r="A80" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2078,34 +1906,34 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="18" t="s">
-        <v>100</v>
+      <c r="A4" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2138,192 +1966,192 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" t="s">
         <v>170</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>171</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>172</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>173</v>
-      </c>
-      <c r="E1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:26">
       <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="B7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="B8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="B10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="B11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -2331,431 +2159,431 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="B13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F13" t="s">
-        <v>47</v>
-      </c>
-      <c r="T13" s="17"/>
-      <c r="Z13" s="17"/>
+        <v>45</v>
+      </c>
+      <c r="T13" s="6"/>
+      <c r="Z13" s="6"/>
     </row>
     <row r="14" spans="1:26">
       <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" t="s">
         <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>125</v>
-      </c>
-      <c r="D14" t="s">
-        <v>53</v>
-      </c>
-      <c r="E14" t="s">
-        <v>126</v>
-      </c>
-      <c r="F14" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="B15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="B16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>132</v>
+      </c>
+      <c r="F18" t="s">
         <v>61</v>
-      </c>
-      <c r="C18" t="s">
-        <v>133</v>
-      </c>
-      <c r="D18" t="s">
-        <v>62</v>
-      </c>
-      <c r="E18" t="s">
-        <v>134</v>
-      </c>
-      <c r="F18" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="2:6">
       <c r="B25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E25" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C27" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E27" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C28" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C29" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E30" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E32" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="B33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E33" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="B34" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C34" t="s">
+        <v>161</v>
+      </c>
+      <c r="D34" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" t="s">
         <v>163</v>
       </c>
-      <c r="D34" t="s">
-        <v>94</v>
-      </c>
-      <c r="E34" t="s">
-        <v>165</v>
-      </c>
       <c r="F34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="B35" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D35" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E35" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="B36" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C36" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E36" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tab name must be "MutationTable" to be parsed in the python code.
</commit_message>
<xml_diff>
--- a/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
+++ b/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="300" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="920" yWindow="0" windowWidth="27380" windowHeight="16120" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Alascca table of mutation class" sheetId="1" r:id="rId1"/>
+    <sheet name="MutationTable" sheetId="1" r:id="rId1"/>
     <sheet name="Version notes" sheetId="2" r:id="rId2"/>
     <sheet name="consequence_types" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -682,8 +682,76 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="189">
+  <cellStyleXfs count="257">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -910,7 +978,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="189">
+  <cellStyles count="257">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1005,6 +1073,40 @@
     <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1099,6 +1201,40 @@
     <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1494,7 +1630,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="94.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Leave "Feature" field blank to specify NA, instead of writing NA explicitly.
</commit_message>
<xml_diff>
--- a/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
+++ b/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="186">
   <si>
     <t>Gene</t>
   </si>
@@ -549,9 +549,6 @@
   </si>
   <si>
     <t>ENSG00000167244</t>
-  </si>
-  <si>
-    <t>NA</t>
   </si>
   <si>
     <t>C124S,G129E,R130G,R130Q</t>
@@ -1625,7 +1622,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1646,7 +1643,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1655,10 +1652,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1671,18 +1668,16 @@
       <c r="C2" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>176</v>
-      </c>
+      <c r="D2" s="9"/>
       <c r="E2" s="11"/>
       <c r="F2" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I2"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>4</v>
@@ -1695,13 +1690,13 @@
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I3"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>4</v>
@@ -1714,7 +1709,7 @@
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I4"/>
     </row>
@@ -1732,16 +1727,16 @@
         <v>6</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I5"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>7</v>
@@ -1756,7 +1751,7 @@
         <v>15</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I6"/>
     </row>
@@ -1777,7 +1772,7 @@
         <v>31</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I7"/>
     </row>
@@ -1798,7 +1793,7 @@
         <v>14</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="I8"/>
     </row>
@@ -1819,7 +1814,7 @@
         <v>13</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I9"/>
     </row>

</xml_diff>

<commit_message>
loss of heterozygosity should be a "B 2" event, as it is not sufficient to ablate PTEN activity by itself.
</commit_message>
<xml_diff>
--- a/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
+++ b/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
@@ -44,6 +44,9 @@
     <t>ENST00000371953</t>
   </si>
   <si>
+    <t>homozygous_loss</t>
+  </si>
+  <si>
     <t>PIK3R1</t>
   </si>
   <si>
@@ -563,22 +566,19 @@
     <t>Flag</t>
   </si>
   <si>
-    <t>ALASSCA_CLASS_B_1</t>
-  </si>
-  <si>
-    <t>ALASSCA_CLASS_A</t>
-  </si>
-  <si>
-    <t>ALASSCA_CLASS_B_2</t>
-  </si>
-  <si>
-    <t>start_lost,stop_gained,frameshift_variant,splice_acceptor_variant,splice_donor_variant</t>
-  </si>
-  <si>
-    <t>loss_of_heterozygosity,homozygous_loss</t>
-  </si>
-  <si>
     <t>frameshift_variant,inframe_insertion,inframe_deletion,stop_gained,splice_acceptor_variant,splice_donor_variant</t>
+  </si>
+  <si>
+    <t>ALASCCA_CLASS_B_1</t>
+  </si>
+  <si>
+    <t>ALASCCA_CLASS_B_2</t>
+  </si>
+  <si>
+    <t>ALASCCA_CLASS_A</t>
+  </si>
+  <si>
+    <t>start_lost,stop_gained,frameshift_variant,splice_acceptor_variant,splice_donor_variant,loss_of_heterozygosity</t>
   </si>
 </sst>
 </file>
@@ -679,8 +679,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="257">
+  <cellStyleXfs count="291">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -975,7 +1009,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="257">
+  <cellStyles count="291">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1104,6 +1138,23 @@
     <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1232,6 +1283,23 @@
     <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1622,7 +1690,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1643,7 +1711,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1652,32 +1720,32 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="11"/>
       <c r="F2" s="9" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I2"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>4</v>
@@ -1690,13 +1758,13 @@
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="I3"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="10" t="s">
-        <v>184</v>
+        <v>7</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>4</v>
@@ -1709,7 +1777,7 @@
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="10" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I4"/>
     </row>
@@ -1727,31 +1795,31 @@
         <v>6</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I5"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="13" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I6"/>
     </row>
@@ -1760,19 +1828,19 @@
         <v>3</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I7"/>
     </row>
@@ -1781,19 +1849,19 @@
         <v>3</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="I8"/>
     </row>
@@ -1802,19 +1870,19 @@
         <v>3</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="I9"/>
     </row>
@@ -2037,34 +2105,34 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
         <v>98</v>
-      </c>
-      <c r="B4" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2097,192 +2165,192 @@
   <sheetData>
     <row r="1" spans="1:26">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:26">
       <c r="B2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" t="s">
         <v>35</v>
-      </c>
-      <c r="E3" t="s">
-        <v>102</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:26">
       <c r="B6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:26">
       <c r="B7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="B9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="B10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:26">
       <c r="B11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" t="s">
         <v>46</v>
-      </c>
-      <c r="E11" t="s">
-        <v>118</v>
-      </c>
-      <c r="F11" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -2290,431 +2358,431 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:26">
       <c r="B13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F13" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="T13" s="6"/>
       <c r="Z13" s="6"/>
     </row>
     <row r="14" spans="1:26">
       <c r="B14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:26">
       <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" t="s">
+        <v>127</v>
+      </c>
+      <c r="F15" t="s">
         <v>53</v>
-      </c>
-      <c r="C15" t="s">
-        <v>125</v>
-      </c>
-      <c r="D15" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" t="s">
-        <v>126</v>
-      </c>
-      <c r="F15" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:26">
       <c r="B16" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" t="s">
+        <v>135</v>
+      </c>
+      <c r="F19" t="s">
         <v>62</v>
-      </c>
-      <c r="C19" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" t="s">
-        <v>134</v>
-      </c>
-      <c r="F19" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D20" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E21" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E22" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C24" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E24" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="2:6">
       <c r="B25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C25" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F25" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E26" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E28" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
+        <v>154</v>
+      </c>
+      <c r="D29" t="s">
         <v>82</v>
       </c>
-      <c r="C29" t="s">
-        <v>153</v>
-      </c>
-      <c r="D29" t="s">
-        <v>81</v>
-      </c>
       <c r="E29" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C30" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D30" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E30" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D31" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E31" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F31" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D32" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E32" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="B33" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E33" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F33" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="B34" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C34" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D34" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E34" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F34" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="B35" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D35" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E35" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F35" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="B36" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C36" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D36" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E36" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F36" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Using three-letter codes for amino acids.
</commit_message>
<xml_diff>
--- a/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
+++ b/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="0" windowWidth="27380" windowHeight="16120" tabRatio="500"/>
+    <workbookView xWindow="320" yWindow="0" windowWidth="27380" windowHeight="16120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="MutationTable" sheetId="1" r:id="rId1"/>
@@ -554,9 +554,6 @@
     <t>ENSG00000167244</t>
   </si>
   <si>
-    <t>C124S,G129E,R130G,R130Q</t>
-  </si>
-  <si>
     <t>Amino_acid_changes</t>
   </si>
   <si>
@@ -579,6 +576,9 @@
   </si>
   <si>
     <t>start_lost,stop_gained,frameshift_variant,splice_acceptor_variant,splice_donor_variant,loss_of_heterozygosity</t>
+  </si>
+  <si>
+    <t>Cys124Ser,Gly129Glu,Arg130Gly,Arg130Gln</t>
   </si>
 </sst>
 </file>
@@ -1690,7 +1690,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1711,7 +1711,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1720,10 +1720,10 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1739,13 +1739,13 @@
       <c r="D2" s="9"/>
       <c r="E2" s="11"/>
       <c r="F2" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I2"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>4</v>
@@ -1758,7 +1758,7 @@
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I3"/>
     </row>
@@ -1777,7 +1777,7 @@
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I4"/>
     </row>
@@ -1795,16 +1795,16 @@
         <v>6</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I5"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>8</v>
@@ -1819,7 +1819,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I6"/>
     </row>
@@ -1840,7 +1840,7 @@
         <v>32</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I7"/>
     </row>
@@ -1861,7 +1861,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I8"/>
     </row>
@@ -1882,7 +1882,7 @@
         <v>14</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I9"/>
     </row>

</xml_diff>

<commit_message>
Changing to using HGVSp strings (e.g. p.Glu68Pro), in both the rule definitions and the internal logic.
</commit_message>
<xml_diff>
--- a/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
+++ b/ALASCCA_MUTATION_TABLE_SPECIFIC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="0" windowWidth="27380" windowHeight="16120" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="MutationTable" sheetId="1" r:id="rId1"/>
@@ -578,7 +578,7 @@
     <t>start_lost,stop_gained,frameshift_variant,splice_acceptor_variant,splice_donor_variant,loss_of_heterozygosity</t>
   </si>
   <si>
-    <t>Cys124Ser,Gly129Glu,Arg130Gly,Arg130Gln</t>
+    <t>p.Cys124Ser,p.Gly129Glu,p.Arg130Gly,p.Arg130Gln</t>
   </si>
 </sst>
 </file>

</xml_diff>